<commit_message>
Data extraction of rows to column implemented
</commit_message>
<xml_diff>
--- a/src/EPPlus.DataExtractor.Tests/spreadsheets/WorkbookTest.xlsx
+++ b/src/EPPlus.DataExtractor.Tests/spreadsheets/WorkbookTest.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Cars list</t>
   </si>
@@ -48,39 +48,6 @@
   </si>
   <si>
     <t>Age</t>
-  </si>
-  <si>
-    <t>Janurary-2016</t>
-  </si>
-  <si>
-    <t>Feburary-2016</t>
-  </si>
-  <si>
-    <t>March-2016</t>
-  </si>
-  <si>
-    <t>April-2016</t>
-  </si>
-  <si>
-    <t>May-2016</t>
-  </si>
-  <si>
-    <t>June-2016</t>
-  </si>
-  <si>
-    <t>July-2016</t>
-  </si>
-  <si>
-    <t>August-2016</t>
-  </si>
-  <si>
-    <t>October-2016</t>
-  </si>
-  <si>
-    <t>November-2016</t>
-  </si>
-  <si>
-    <t>December-2016</t>
   </si>
   <si>
     <t>John</t>
@@ -465,102 +432,113 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:R11"/>
+  <dimension ref="B1:S11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="16" max="16" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15" customWidth="1"/>
+    <col min="19" max="19" width="16" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="H1" s="8">
+        <v>42370</v>
+      </c>
+      <c r="I1" s="8">
+        <v>42401</v>
+      </c>
+      <c r="J1" s="8">
+        <v>42430</v>
+      </c>
+      <c r="K1" s="8">
+        <v>42461</v>
+      </c>
+      <c r="L1" s="8">
+        <v>42491</v>
+      </c>
+      <c r="M1" s="8">
+        <v>42522</v>
+      </c>
+      <c r="N1" s="8">
+        <v>42552</v>
+      </c>
+      <c r="O1" s="8">
+        <v>42583</v>
+      </c>
+      <c r="P1" s="8">
+        <v>42614</v>
+      </c>
+      <c r="Q1" s="8">
+        <v>42644</v>
+      </c>
+      <c r="R1" s="8">
+        <v>42675</v>
+      </c>
+      <c r="S1" s="8">
+        <v>42705</v>
+      </c>
+    </row>
+    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="F2" s="6" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="G2" s="6">
         <v>32</v>
       </c>
       <c r="H2" s="7">
+        <v>10</v>
+      </c>
+      <c r="I2" s="7">
         <v>3750</v>
       </c>
-      <c r="I2" s="7">
+      <c r="J2" s="7">
         <v>780</v>
       </c>
-      <c r="J2" s="7">
+      <c r="K2" s="7">
         <v>5400</v>
       </c>
-      <c r="K2" s="7">
+      <c r="L2" s="7">
         <v>2890</v>
       </c>
-      <c r="L2" s="7">
-        <v>1</v>
-      </c>
       <c r="M2" s="7">
+        <v>1</v>
+      </c>
+      <c r="N2" s="7">
         <v>2</v>
       </c>
-      <c r="N2" s="7">
+      <c r="O2" s="7">
         <v>3</v>
       </c>
-      <c r="O2" s="7">
-        <v>4</v>
-      </c>
       <c r="P2" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="7">
         <v>5</v>
       </c>
-      <c r="Q2" s="7">
+      <c r="R2" s="7">
         <v>6</v>
       </c>
-      <c r="R2" s="7">
+      <c r="S2" s="7">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -571,13 +549,13 @@
         <v>6</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G3" s="6">
         <v>56</v>
       </c>
       <c r="H3" s="7">
-        <v>13000</v>
+        <v>11</v>
       </c>
       <c r="I3" s="7">
         <v>13000</v>
@@ -592,11 +570,11 @@
         <v>13000</v>
       </c>
       <c r="M3" s="7">
+        <v>13000</v>
+      </c>
+      <c r="N3" s="7">
         <v>17560</v>
       </c>
-      <c r="N3" s="7">
-        <v>13000</v>
-      </c>
       <c r="O3" s="7">
         <v>13000</v>
       </c>
@@ -607,10 +585,13 @@
         <v>13000</v>
       </c>
       <c r="R3" s="7">
+        <v>13000</v>
+      </c>
+      <c r="S3" s="7">
         <v>19870</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -621,13 +602,13 @@
         <v>42917</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="G4" s="6">
         <v>45</v>
       </c>
       <c r="H4" s="7">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="I4" s="7">
         <v>1</v>
@@ -659,8 +640,11 @@
       <c r="R4" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="S4" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -670,7 +654,6 @@
       <c r="D5" s="3">
         <v>42840</v>
       </c>
-      <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
@@ -681,8 +664,9 @@
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="S5" s="5"/>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -692,7 +676,6 @@
       <c r="D6" s="3">
         <v>42206</v>
       </c>
-      <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
@@ -703,20 +686,21 @@
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="S6" s="5"/>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="D11" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added option for getting value object through a custom function
</commit_message>
<xml_diff>
--- a/src/EPPlus.DataExtractor.Tests/spreadsheets/WorkbookTest.xlsx
+++ b/src/EPPlus.DataExtractor.Tests/spreadsheets/WorkbookTest.xlsx
@@ -13,6 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="MainWorksheet" sheetId="1" r:id="rId1"/>
+    <sheet name="SecondaryWorksheet" sheetId="3" r:id="rId2"/>
+    <sheet name="TablesWorksheet" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
   <si>
     <t>Cars list</t>
   </si>
@@ -57,19 +59,121 @@
   </si>
   <si>
     <t>Mary</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>Cleiton</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Joseph</t>
+  </si>
+  <si>
+    <t>Greg</t>
+  </si>
+  <si>
+    <t>Hudson</t>
+  </si>
+  <si>
+    <t>Francis</t>
+  </si>
+  <si>
+    <t>Wanessa</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Money received</t>
+  </si>
+  <si>
+    <t>Money spent</t>
+  </si>
+  <si>
+    <t>Goal</t>
+  </si>
+  <si>
+    <t>Effective</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Expenses</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Indicators</t>
+  </si>
+  <si>
+    <t>São Paulo (BR)</t>
+  </si>
+  <si>
+    <t>New York (US)</t>
+  </si>
+  <si>
+    <t>London (UK)</t>
+  </si>
+  <si>
+    <t>Jan-10</t>
+  </si>
+  <si>
+    <t>Feb-10</t>
+  </si>
+  <si>
+    <t>Mar-10</t>
+  </si>
+  <si>
+    <t>Apr-10</t>
+  </si>
+  <si>
+    <t>May-10</t>
+  </si>
+  <si>
+    <t>Jun-10</t>
+  </si>
+  <si>
+    <t>Jul-10</t>
+  </si>
+  <si>
+    <t>Aug-10</t>
+  </si>
+  <si>
+    <t>Sep-10</t>
+  </si>
+  <si>
+    <t>Oct-10</t>
+  </si>
+  <si>
+    <t>Nov-10</t>
+  </si>
+  <si>
+    <t>Dec-10</t>
+  </si>
+  <si>
+    <t>Effective / Goal %</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="4">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
     <numFmt numFmtId="165" formatCode="[$$-1009]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="[$$-409]#,##0.00"/>
     <numFmt numFmtId="167" formatCode="[$-409]mmmm\-yy;@"/>
+    <numFmt numFmtId="168" formatCode="[$€-2]\ #,##0.00"/>
+    <numFmt numFmtId="169" formatCode="[$€-1809]#,##0.00"/>
+    <numFmt numFmtId="170" formatCode="[$-409]mmm\-yy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,16 +189,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -102,11 +219,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -115,14 +285,172 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Celda de comprobación" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="17">
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$€-2]\ #,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="[$-409]mmmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="[$€-1809]#,##0.00"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="[$-409]mmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -133,6 +461,50 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="D1:O19" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="D1:O19"/>
+  <tableColumns count="12">
+    <tableColumn id="1" name="Jan-10"/>
+    <tableColumn id="2" name="Feb-10"/>
+    <tableColumn id="3" name="Mar-10"/>
+    <tableColumn id="4" name="Apr-10"/>
+    <tableColumn id="5" name="May-10"/>
+    <tableColumn id="6" name="Jun-10"/>
+    <tableColumn id="7" name="Jul-10"/>
+    <tableColumn id="8" name="Aug-10"/>
+    <tableColumn id="9" name="Sep-10"/>
+    <tableColumn id="10" name="Oct-10"/>
+    <tableColumn id="11" name="Nov-10"/>
+    <tableColumn id="12" name="Dec-10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="C3:D11" totalsRowShown="0">
+  <autoFilter ref="C3:D11"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Name"/>
+    <tableColumn id="2" name="Age"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="G1:I13" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="G1:I13"/>
+  <tableColumns count="3">
+    <tableColumn id="3" name="Money spent" dataDxfId="2"/>
+    <tableColumn id="1" name="Date" dataDxfId="1"/>
+    <tableColumn id="2" name="Money received" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -435,7 +807,7 @@
   <dimension ref="B1:S11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,11 +864,11 @@
       </c>
     </row>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
       <c r="F2" s="5" t="s">
         <v>8</v>
       </c>
@@ -607,7 +979,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="5">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="H4" s="6">
         <v>12</v>
@@ -712,4 +1084,1233 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2">
+        <v>250</v>
+      </c>
+      <c r="E2">
+        <v>245</v>
+      </c>
+      <c r="F2">
+        <v>190</v>
+      </c>
+      <c r="G2">
+        <v>180</v>
+      </c>
+      <c r="H2">
+        <v>190</v>
+      </c>
+      <c r="I2">
+        <v>200</v>
+      </c>
+      <c r="J2">
+        <v>120</v>
+      </c>
+      <c r="K2">
+        <v>150</v>
+      </c>
+      <c r="L2">
+        <v>160</v>
+      </c>
+      <c r="M2">
+        <v>200</v>
+      </c>
+      <c r="N2">
+        <v>500</v>
+      </c>
+      <c r="O2">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="17"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3">
+        <v>270</v>
+      </c>
+      <c r="E3">
+        <v>200</v>
+      </c>
+      <c r="F3">
+        <v>200</v>
+      </c>
+      <c r="G3">
+        <v>180</v>
+      </c>
+      <c r="H3">
+        <v>180</v>
+      </c>
+      <c r="I3">
+        <v>178</v>
+      </c>
+      <c r="J3">
+        <v>245</v>
+      </c>
+      <c r="K3">
+        <v>190</v>
+      </c>
+      <c r="L3">
+        <v>150</v>
+      </c>
+      <c r="M3">
+        <v>290</v>
+      </c>
+      <c r="N3">
+        <v>987</v>
+      </c>
+      <c r="O3">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="17"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="14">
+        <f>(D3/D2)</f>
+        <v>1.08</v>
+      </c>
+      <c r="E4" s="14">
+        <f t="shared" ref="E4:O4" si="0">(E3/E2)</f>
+        <v>0.81632653061224492</v>
+      </c>
+      <c r="F4" s="14">
+        <f t="shared" si="0"/>
+        <v>1.0526315789473684</v>
+      </c>
+      <c r="G4" s="14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H4" s="14">
+        <f t="shared" si="0"/>
+        <v>0.94736842105263153</v>
+      </c>
+      <c r="I4" s="14">
+        <f t="shared" si="0"/>
+        <v>0.89</v>
+      </c>
+      <c r="J4" s="14">
+        <f t="shared" si="0"/>
+        <v>2.0416666666666665</v>
+      </c>
+      <c r="K4" s="14">
+        <f t="shared" si="0"/>
+        <v>1.2666666666666666</v>
+      </c>
+      <c r="L4" s="14">
+        <f t="shared" si="0"/>
+        <v>0.9375</v>
+      </c>
+      <c r="M4" s="14">
+        <f t="shared" si="0"/>
+        <v>1.45</v>
+      </c>
+      <c r="N4" s="14">
+        <f t="shared" si="0"/>
+        <v>1.974</v>
+      </c>
+      <c r="O4" s="14">
+        <f t="shared" si="0"/>
+        <v>1.2985074626865671</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="17"/>
+      <c r="B5" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>250</v>
+      </c>
+      <c r="E5">
+        <v>245</v>
+      </c>
+      <c r="F5">
+        <v>190</v>
+      </c>
+      <c r="G5">
+        <v>180</v>
+      </c>
+      <c r="H5">
+        <v>190</v>
+      </c>
+      <c r="I5">
+        <v>200</v>
+      </c>
+      <c r="J5">
+        <v>120</v>
+      </c>
+      <c r="K5">
+        <v>150</v>
+      </c>
+      <c r="L5">
+        <v>160</v>
+      </c>
+      <c r="M5">
+        <v>200</v>
+      </c>
+      <c r="N5">
+        <v>500</v>
+      </c>
+      <c r="O5">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="17"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6">
+        <v>270</v>
+      </c>
+      <c r="E6">
+        <v>200</v>
+      </c>
+      <c r="F6">
+        <v>200</v>
+      </c>
+      <c r="G6">
+        <v>180</v>
+      </c>
+      <c r="H6">
+        <v>180</v>
+      </c>
+      <c r="I6">
+        <v>178</v>
+      </c>
+      <c r="J6">
+        <v>245</v>
+      </c>
+      <c r="K6">
+        <v>190</v>
+      </c>
+      <c r="L6">
+        <v>150</v>
+      </c>
+      <c r="M6">
+        <v>290</v>
+      </c>
+      <c r="N6">
+        <v>987</v>
+      </c>
+      <c r="O6">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="18"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="14">
+        <f>D6/D5</f>
+        <v>1.08</v>
+      </c>
+      <c r="E7" s="14">
+        <f t="shared" ref="E7:O7" si="1">E6/E5</f>
+        <v>0.81632653061224492</v>
+      </c>
+      <c r="F7" s="14">
+        <f t="shared" si="1"/>
+        <v>1.0526315789473684</v>
+      </c>
+      <c r="G7" s="14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H7" s="14">
+        <f t="shared" si="1"/>
+        <v>0.94736842105263153</v>
+      </c>
+      <c r="I7" s="14">
+        <f t="shared" si="1"/>
+        <v>0.89</v>
+      </c>
+      <c r="J7" s="14">
+        <f t="shared" si="1"/>
+        <v>2.0416666666666665</v>
+      </c>
+      <c r="K7" s="14">
+        <f t="shared" si="1"/>
+        <v>1.2666666666666666</v>
+      </c>
+      <c r="L7" s="14">
+        <f t="shared" si="1"/>
+        <v>0.9375</v>
+      </c>
+      <c r="M7" s="14">
+        <f t="shared" si="1"/>
+        <v>1.45</v>
+      </c>
+      <c r="N7" s="14">
+        <f t="shared" si="1"/>
+        <v>1.974</v>
+      </c>
+      <c r="O7" s="14">
+        <f t="shared" si="1"/>
+        <v>1.2985074626865671</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8">
+        <v>200</v>
+      </c>
+      <c r="E8">
+        <v>200</v>
+      </c>
+      <c r="F8">
+        <v>170</v>
+      </c>
+      <c r="G8">
+        <v>145</v>
+      </c>
+      <c r="H8">
+        <v>145</v>
+      </c>
+      <c r="I8">
+        <v>140</v>
+      </c>
+      <c r="J8">
+        <v>100</v>
+      </c>
+      <c r="K8">
+        <v>110</v>
+      </c>
+      <c r="L8">
+        <v>110</v>
+      </c>
+      <c r="M8">
+        <v>160</v>
+      </c>
+      <c r="N8">
+        <v>350</v>
+      </c>
+      <c r="O8">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="17"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9">
+        <v>200</v>
+      </c>
+      <c r="E9">
+        <v>200</v>
+      </c>
+      <c r="F9">
+        <v>170</v>
+      </c>
+      <c r="G9">
+        <v>145</v>
+      </c>
+      <c r="H9">
+        <v>145</v>
+      </c>
+      <c r="I9">
+        <v>150</v>
+      </c>
+      <c r="J9">
+        <v>110</v>
+      </c>
+      <c r="K9">
+        <v>120</v>
+      </c>
+      <c r="L9">
+        <v>130</v>
+      </c>
+      <c r="M9">
+        <v>150</v>
+      </c>
+      <c r="N9">
+        <v>330</v>
+      </c>
+      <c r="O9">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="17"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="14">
+        <f>D9/D8</f>
+        <v>1</v>
+      </c>
+      <c r="E10" s="14">
+        <f t="shared" ref="E10:O10" si="2">E9/E8</f>
+        <v>1</v>
+      </c>
+      <c r="F10" s="14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G10" s="14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H10" s="14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I10" s="14">
+        <f t="shared" si="2"/>
+        <v>1.0714285714285714</v>
+      </c>
+      <c r="J10" s="14">
+        <f t="shared" si="2"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K10" s="14">
+        <f t="shared" si="2"/>
+        <v>1.0909090909090908</v>
+      </c>
+      <c r="L10" s="14">
+        <f t="shared" si="2"/>
+        <v>1.1818181818181819</v>
+      </c>
+      <c r="M10" s="14">
+        <f t="shared" si="2"/>
+        <v>0.9375</v>
+      </c>
+      <c r="N10" s="14">
+        <f t="shared" si="2"/>
+        <v>0.94285714285714284</v>
+      </c>
+      <c r="O10" s="14">
+        <f t="shared" si="2"/>
+        <v>0.874</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="17"/>
+      <c r="B11" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11">
+        <v>100</v>
+      </c>
+      <c r="E11">
+        <v>100</v>
+      </c>
+      <c r="F11">
+        <v>100</v>
+      </c>
+      <c r="G11">
+        <v>100</v>
+      </c>
+      <c r="H11">
+        <v>100</v>
+      </c>
+      <c r="I11">
+        <v>100</v>
+      </c>
+      <c r="J11">
+        <v>120</v>
+      </c>
+      <c r="K11">
+        <v>100</v>
+      </c>
+      <c r="L11">
+        <v>100</v>
+      </c>
+      <c r="M11">
+        <v>100</v>
+      </c>
+      <c r="N11">
+        <v>120</v>
+      </c>
+      <c r="O11">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="17"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12">
+        <v>80</v>
+      </c>
+      <c r="E12">
+        <v>80</v>
+      </c>
+      <c r="F12">
+        <v>90</v>
+      </c>
+      <c r="G12">
+        <v>90</v>
+      </c>
+      <c r="H12">
+        <v>98</v>
+      </c>
+      <c r="I12">
+        <v>97</v>
+      </c>
+      <c r="J12">
+        <v>130</v>
+      </c>
+      <c r="K12">
+        <v>90</v>
+      </c>
+      <c r="L12">
+        <v>78</v>
+      </c>
+      <c r="M12">
+        <v>80</v>
+      </c>
+      <c r="N12">
+        <v>95</v>
+      </c>
+      <c r="O12">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="18"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="14">
+        <f>D12/D11</f>
+        <v>0.8</v>
+      </c>
+      <c r="E13" s="14">
+        <f t="shared" ref="E13:O13" si="3">E12/E11</f>
+        <v>0.8</v>
+      </c>
+      <c r="F13" s="14">
+        <f t="shared" si="3"/>
+        <v>0.9</v>
+      </c>
+      <c r="G13" s="14">
+        <f t="shared" si="3"/>
+        <v>0.9</v>
+      </c>
+      <c r="H13" s="14">
+        <f t="shared" si="3"/>
+        <v>0.98</v>
+      </c>
+      <c r="I13" s="14">
+        <f t="shared" si="3"/>
+        <v>0.97</v>
+      </c>
+      <c r="J13" s="14">
+        <f t="shared" si="3"/>
+        <v>1.0833333333333333</v>
+      </c>
+      <c r="K13" s="14">
+        <f t="shared" si="3"/>
+        <v>0.9</v>
+      </c>
+      <c r="L13" s="14">
+        <f t="shared" si="3"/>
+        <v>0.78</v>
+      </c>
+      <c r="M13" s="14">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
+      <c r="N13" s="14">
+        <f t="shared" si="3"/>
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="O13" s="14">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14">
+        <v>250</v>
+      </c>
+      <c r="E14">
+        <v>245</v>
+      </c>
+      <c r="F14">
+        <v>190</v>
+      </c>
+      <c r="G14">
+        <v>180</v>
+      </c>
+      <c r="H14">
+        <v>190</v>
+      </c>
+      <c r="I14">
+        <v>200</v>
+      </c>
+      <c r="J14">
+        <v>120</v>
+      </c>
+      <c r="K14">
+        <v>150</v>
+      </c>
+      <c r="L14">
+        <v>160</v>
+      </c>
+      <c r="M14">
+        <v>200</v>
+      </c>
+      <c r="N14">
+        <v>500</v>
+      </c>
+      <c r="O14">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="17"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15">
+        <v>270</v>
+      </c>
+      <c r="E15">
+        <v>200</v>
+      </c>
+      <c r="F15">
+        <v>200</v>
+      </c>
+      <c r="G15">
+        <v>180</v>
+      </c>
+      <c r="H15">
+        <v>180</v>
+      </c>
+      <c r="I15">
+        <v>178</v>
+      </c>
+      <c r="J15">
+        <v>245</v>
+      </c>
+      <c r="K15">
+        <v>190</v>
+      </c>
+      <c r="L15">
+        <v>150</v>
+      </c>
+      <c r="M15">
+        <v>290</v>
+      </c>
+      <c r="N15">
+        <v>987</v>
+      </c>
+      <c r="O15">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="17"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="14">
+        <f>D15/D14</f>
+        <v>1.08</v>
+      </c>
+      <c r="E16" s="14">
+        <f t="shared" ref="E16:O16" si="4">E15/E14</f>
+        <v>0.81632653061224492</v>
+      </c>
+      <c r="F16" s="14">
+        <f t="shared" si="4"/>
+        <v>1.0526315789473684</v>
+      </c>
+      <c r="G16" s="14">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="H16" s="14">
+        <f t="shared" si="4"/>
+        <v>0.94736842105263153</v>
+      </c>
+      <c r="I16" s="14">
+        <f t="shared" si="4"/>
+        <v>0.89</v>
+      </c>
+      <c r="J16" s="14">
+        <f t="shared" si="4"/>
+        <v>2.0416666666666665</v>
+      </c>
+      <c r="K16" s="14">
+        <f t="shared" si="4"/>
+        <v>1.2666666666666666</v>
+      </c>
+      <c r="L16" s="14">
+        <f t="shared" si="4"/>
+        <v>0.9375</v>
+      </c>
+      <c r="M16" s="14">
+        <f t="shared" si="4"/>
+        <v>1.45</v>
+      </c>
+      <c r="N16" s="14">
+        <f t="shared" si="4"/>
+        <v>1.974</v>
+      </c>
+      <c r="O16" s="14">
+        <f t="shared" si="4"/>
+        <v>1.2985074626865671</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="17"/>
+      <c r="B17" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17">
+        <v>250</v>
+      </c>
+      <c r="E17">
+        <v>245</v>
+      </c>
+      <c r="F17">
+        <v>190</v>
+      </c>
+      <c r="G17">
+        <v>180</v>
+      </c>
+      <c r="H17">
+        <v>190</v>
+      </c>
+      <c r="I17">
+        <v>200</v>
+      </c>
+      <c r="J17">
+        <v>120</v>
+      </c>
+      <c r="K17">
+        <v>150</v>
+      </c>
+      <c r="L17">
+        <v>160</v>
+      </c>
+      <c r="M17">
+        <v>200</v>
+      </c>
+      <c r="N17">
+        <v>500</v>
+      </c>
+      <c r="O17">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="17"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18">
+        <v>270</v>
+      </c>
+      <c r="E18">
+        <v>200</v>
+      </c>
+      <c r="F18">
+        <v>200</v>
+      </c>
+      <c r="G18">
+        <v>180</v>
+      </c>
+      <c r="H18">
+        <v>180</v>
+      </c>
+      <c r="I18">
+        <v>178</v>
+      </c>
+      <c r="J18">
+        <v>245</v>
+      </c>
+      <c r="K18">
+        <v>190</v>
+      </c>
+      <c r="L18">
+        <v>150</v>
+      </c>
+      <c r="M18">
+        <v>290</v>
+      </c>
+      <c r="N18">
+        <v>987</v>
+      </c>
+      <c r="O18">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="18"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="14">
+        <f>D18/D17</f>
+        <v>1.08</v>
+      </c>
+      <c r="E19" s="14">
+        <f t="shared" ref="E19:O19" si="5">E18/E17</f>
+        <v>0.81632653061224492</v>
+      </c>
+      <c r="F19" s="14">
+        <f t="shared" si="5"/>
+        <v>1.0526315789473684</v>
+      </c>
+      <c r="G19" s="14">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H19" s="14">
+        <f t="shared" si="5"/>
+        <v>0.94736842105263153</v>
+      </c>
+      <c r="I19" s="14">
+        <f t="shared" si="5"/>
+        <v>0.89</v>
+      </c>
+      <c r="J19" s="14">
+        <f t="shared" si="5"/>
+        <v>2.0416666666666665</v>
+      </c>
+      <c r="K19" s="14">
+        <f t="shared" si="5"/>
+        <v>1.2666666666666666</v>
+      </c>
+      <c r="L19" s="14">
+        <f t="shared" si="5"/>
+        <v>0.9375</v>
+      </c>
+      <c r="M19" s="14">
+        <f t="shared" si="5"/>
+        <v>1.45</v>
+      </c>
+      <c r="N19" s="14">
+        <f t="shared" si="5"/>
+        <v>1.974</v>
+      </c>
+      <c r="O19" s="14">
+        <f t="shared" si="5"/>
+        <v>1.2985074626865671</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D4:O4">
+    <cfRule type="cellIs" dxfId="16" priority="12" operator="greaterThan">
+      <formula>0.98</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="11" operator="lessThan">
+      <formula>0.98</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7:O7">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="lessThanOrEqual">
+      <formula>0.98</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="9" operator="greaterThan">
+      <formula>0.98</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10:O10">
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="greaterThan">
+      <formula>0.98</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="lessThan">
+      <formula>0.98</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13:O13">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="lessThanOrEqual">
+      <formula>0.98</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="greaterThan">
+      <formula>0.98</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16:O16">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="greaterThanOrEqual">
+      <formula>0.98</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="lessThan">
+      <formula>0.98</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D19:O19">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="lessThanOrEqual">
+      <formula>0.98</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+      <formula>0.98</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C1:I13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="4" width="12" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F2" s="10"/>
+      <c r="G2" s="10">
+        <v>500</v>
+      </c>
+      <c r="H2" s="9">
+        <v>42370</v>
+      </c>
+      <c r="I2" s="8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10">
+        <v>450</v>
+      </c>
+      <c r="H3" s="9">
+        <v>42401</v>
+      </c>
+      <c r="I3" s="8">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>35</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10">
+        <v>300</v>
+      </c>
+      <c r="H4" s="9">
+        <v>42430</v>
+      </c>
+      <c r="I4" s="8">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>57</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10">
+        <v>300</v>
+      </c>
+      <c r="H5" s="9">
+        <v>42461</v>
+      </c>
+      <c r="I5" s="8">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>43</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10">
+        <v>340</v>
+      </c>
+      <c r="H6" s="9">
+        <v>42491</v>
+      </c>
+      <c r="I6" s="8">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>23</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10">
+        <v>317</v>
+      </c>
+      <c r="H7" s="9">
+        <v>42522</v>
+      </c>
+      <c r="I7" s="8">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>54</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10">
+        <v>400</v>
+      </c>
+      <c r="H8" s="9">
+        <v>42552</v>
+      </c>
+      <c r="I8" s="8">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9">
+        <v>24</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10">
+        <v>290</v>
+      </c>
+      <c r="H9" s="9">
+        <v>42583</v>
+      </c>
+      <c r="I9" s="8">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10">
+        <v>44</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10">
+        <v>307</v>
+      </c>
+      <c r="H10" s="9">
+        <v>42614</v>
+      </c>
+      <c r="I10" s="8">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11">
+        <v>25</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10">
+        <v>280</v>
+      </c>
+      <c r="H11" s="9">
+        <v>42644</v>
+      </c>
+      <c r="I11" s="8">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F12" s="10"/>
+      <c r="G12" s="10">
+        <v>417</v>
+      </c>
+      <c r="H12" s="9">
+        <v>42675</v>
+      </c>
+      <c r="I12" s="8">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F13" s="10"/>
+      <c r="G13" s="10">
+        <v>450</v>
+      </c>
+      <c r="H13" s="9">
+        <v>42705</v>
+      </c>
+      <c r="I13" s="8">
+        <v>1200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added WithCollection method that assumes headerless, simple types
</commit_message>
<xml_diff>
--- a/src/EPPlus.DataExtractor.Tests/spreadsheets/WorkbookTest.xlsx
+++ b/src/EPPlus.DataExtractor.Tests/spreadsheets/WorkbookTest.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perei\Documents\Development\EPPlus.DataExtractor\src\EPPlus.DataExtractor.Tests\spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\EPPlus.DataExtractor\src\EPPlus.DataExtractor.Tests\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14535" windowHeight="5595"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="14535" windowHeight="5595" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="MainWorksheet" sheetId="1" r:id="rId1"/>
     <sheet name="SecondaryWorksheet" sheetId="3" r:id="rId2"/>
     <sheet name="TablesWorksheet" sheetId="2" r:id="rId3"/>
+    <sheet name="StringsCollectionWorksheet" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
   <si>
     <t>Cars list</t>
   </si>
@@ -158,6 +159,33 @@
   </si>
   <si>
     <t>Effective / Goal %</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>LanguagesSpoken1</t>
+  </si>
+  <si>
+    <t>LanguagesSpoken2</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>Romanian</t>
+  </si>
+  <si>
+    <t>Name2</t>
+  </si>
+  <si>
+    <t>English</t>
   </si>
 </sst>
 </file>
@@ -173,7 +201,7 @@
     <numFmt numFmtId="169" formatCode="[$€-1809]#,##0.00"/>
     <numFmt numFmtId="170" formatCode="[$-409]mmm\-yy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,8 +225,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -210,8 +252,14 @@
         <fgColor rgb="FFA5A5A5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -271,12 +319,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -294,7 +372,20 @@
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
@@ -306,12 +397,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Celda de comprobación" xfId="1" builtinId="23"/>
+    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
@@ -329,6 +417,16 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="170" formatCode="[$-409]mmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -437,16 +535,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -806,11 +894,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.42578125" bestFit="1" customWidth="1"/>
@@ -864,11 +952,11 @@
       </c>
     </row>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
       <c r="F2" s="5" t="s">
         <v>8</v>
       </c>
@@ -1094,7 +1182,7 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.5703125" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
@@ -1104,10 +1192,10 @@
       <c r="A1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="19"/>
+      <c r="C1" s="20"/>
       <c r="D1" s="12" t="s">
         <v>31</v>
       </c>
@@ -1146,10 +1234,10 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="20" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="13" t="s">
@@ -1193,8 +1281,8 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17"/>
-      <c r="B3" s="19"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="13" t="s">
         <v>23</v>
       </c>
@@ -1236,8 +1324,8 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
-      <c r="B4" s="19"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="13" t="s">
         <v>43</v>
       </c>
@@ -1291,8 +1379,8 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17"/>
-      <c r="B5" s="19" t="s">
+      <c r="A5" s="22"/>
+      <c r="B5" s="20" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="13" t="s">
@@ -1336,8 +1424,8 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="17"/>
-      <c r="B6" s="19"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="13" t="s">
         <v>23</v>
       </c>
@@ -1379,8 +1467,8 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18"/>
-      <c r="B7" s="19"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="13" t="s">
         <v>43</v>
       </c>
@@ -1434,10 +1522,10 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="20" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="13" t="s">
@@ -1481,8 +1569,8 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
-      <c r="B9" s="19"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="13" t="s">
         <v>23</v>
       </c>
@@ -1524,8 +1612,8 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="17"/>
-      <c r="B10" s="19"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="13" t="s">
         <v>43</v>
       </c>
@@ -1579,8 +1667,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
-      <c r="B11" s="19" t="s">
+      <c r="A11" s="22"/>
+      <c r="B11" s="20" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="13" t="s">
@@ -1624,8 +1712,8 @@
       </c>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
-      <c r="B12" s="19"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="13" t="s">
         <v>23</v>
       </c>
@@ -1667,8 +1755,8 @@
       </c>
     </row>
     <row r="13" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="18"/>
-      <c r="B13" s="19"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="13" t="s">
         <v>43</v>
       </c>
@@ -1722,10 +1810,10 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="20" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="13" t="s">
@@ -1769,8 +1857,8 @@
       </c>
     </row>
     <row r="15" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
-      <c r="B15" s="19"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="13" t="s">
         <v>23</v>
       </c>
@@ -1812,8 +1900,8 @@
       </c>
     </row>
     <row r="16" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
-      <c r="B16" s="19"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="13" t="s">
         <v>43</v>
       </c>
@@ -1867,8 +1955,8 @@
       </c>
     </row>
     <row r="17" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
-      <c r="B17" s="19" t="s">
+      <c r="A17" s="22"/>
+      <c r="B17" s="20" t="s">
         <v>25</v>
       </c>
       <c r="C17" s="13" t="s">
@@ -1912,8 +2000,8 @@
       </c>
     </row>
     <row r="18" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
-      <c r="B18" s="19"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="13" t="s">
         <v>23</v>
       </c>
@@ -1955,8 +2043,8 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="18"/>
-      <c r="B19" s="19"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="13" t="s">
         <v>43</v>
       </c>
@@ -2024,50 +2112,50 @@
     <mergeCell ref="B5:B7"/>
   </mergeCells>
   <conditionalFormatting sqref="D4:O4">
-    <cfRule type="cellIs" dxfId="16" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="11" operator="lessThan">
       <formula>0.98</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="12" operator="greaterThan">
       <formula>0.98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:O7">
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="14" priority="9" operator="greaterThan">
       <formula>0.98</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="lessThanOrEqual">
       <formula>0.98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:O10">
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="lessThan">
       <formula>0.98</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="greaterThan">
       <formula>0.98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13:O13">
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="greaterThan">
       <formula>0.98</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="lessThanOrEqual">
       <formula>0.98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:O16">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="lessThan">
       <formula>0.98</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="greaterThanOrEqual">
       <formula>0.98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19:O19">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
       <formula>0.98</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="lessThanOrEqual">
       <formula>0.98</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2087,7 +2175,7 @@
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="4" width="12" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
@@ -2313,4 +2401,75 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Improving documentation for simple collection
</commit_message>
<xml_diff>
--- a/src/EPPlus.DataExtractor.Tests/spreadsheets/WorkbookTest.xlsx
+++ b/src/EPPlus.DataExtractor.Tests/spreadsheets/WorkbookTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\csharp\EPPlus.DataExtractor\src\EPPlus.DataExtractor.Tests\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838F05AF-374F-42C9-B17A-265B6553C590}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96859B25-C341-4468-92B9-A921A26DFBA1}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14535" windowHeight="5595" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="71">
   <si>
     <t>Cars list</t>
   </si>
@@ -230,6 +230,18 @@
   </si>
   <si>
     <t>English</t>
+  </si>
+  <si>
+    <t>LanguagesSpoken3</t>
+  </si>
+  <si>
+    <t>Mandarin</t>
+  </si>
+  <si>
+    <t>Latin</t>
+  </si>
+  <si>
+    <t>Baby</t>
   </si>
 </sst>
 </file>
@@ -245,7 +257,7 @@
     <numFmt numFmtId="169" formatCode="[$€-1809]#,##0.00"/>
     <numFmt numFmtId="170" formatCode="[$-409]mmm\-yy;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,6 +290,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -404,7 +423,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -425,6 +444,16 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -440,16 +469,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Celda de comprobación" xfId="1" builtinId="23"/>
@@ -1005,11 +1025,11 @@
       </c>
     </row>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
       <c r="F2" s="5" t="s">
         <v>8</v>
       </c>
@@ -1245,10 +1265,10 @@
       <c r="A1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="19"/>
+      <c r="C1" s="23"/>
       <c r="D1" s="12" t="s">
         <v>31</v>
       </c>
@@ -1287,10 +1307,10 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="23" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="13" t="s">
@@ -1334,8 +1354,8 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21"/>
-      <c r="B3" s="19"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="13" t="s">
         <v>23</v>
       </c>
@@ -1377,8 +1397,8 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="21"/>
-      <c r="B4" s="19"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="13" t="s">
         <v>43</v>
       </c>
@@ -1432,8 +1452,8 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="21"/>
-      <c r="B5" s="19" t="s">
+      <c r="A5" s="25"/>
+      <c r="B5" s="23" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="13" t="s">
@@ -1477,8 +1497,8 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="21"/>
-      <c r="B6" s="19"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="13" t="s">
         <v>23</v>
       </c>
@@ -1520,8 +1540,8 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="22"/>
-      <c r="B7" s="19"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="23"/>
       <c r="C7" s="13" t="s">
         <v>43</v>
       </c>
@@ -1575,10 +1595,10 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="23" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="13" t="s">
@@ -1622,8 +1642,8 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="21"/>
-      <c r="B9" s="19"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="23"/>
       <c r="C9" s="13" t="s">
         <v>23</v>
       </c>
@@ -1665,8 +1685,8 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="21"/>
-      <c r="B10" s="19"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="13" t="s">
         <v>43</v>
       </c>
@@ -1720,8 +1740,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="21"/>
-      <c r="B11" s="19" t="s">
+      <c r="A11" s="25"/>
+      <c r="B11" s="23" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="13" t="s">
@@ -1765,8 +1785,8 @@
       </c>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
-      <c r="B12" s="19"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="23"/>
       <c r="C12" s="13" t="s">
         <v>23</v>
       </c>
@@ -1808,8 +1828,8 @@
       </c>
     </row>
     <row r="13" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22"/>
-      <c r="B13" s="19"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="23"/>
       <c r="C13" s="13" t="s">
         <v>43</v>
       </c>
@@ -1863,10 +1883,10 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="23" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="13" t="s">
@@ -1910,8 +1930,8 @@
       </c>
     </row>
     <row r="15" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="21"/>
-      <c r="B15" s="19"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="23"/>
       <c r="C15" s="13" t="s">
         <v>23</v>
       </c>
@@ -1953,8 +1973,8 @@
       </c>
     </row>
     <row r="16" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="21"/>
-      <c r="B16" s="19"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="23"/>
       <c r="C16" s="13" t="s">
         <v>43</v>
       </c>
@@ -2008,8 +2028,8 @@
       </c>
     </row>
     <row r="17" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="21"/>
-      <c r="B17" s="19" t="s">
+      <c r="A17" s="25"/>
+      <c r="B17" s="23" t="s">
         <v>25</v>
       </c>
       <c r="C17" s="13" t="s">
@@ -2053,8 +2073,8 @@
       </c>
     </row>
     <row r="18" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="21"/>
-      <c r="B18" s="19"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="13" t="s">
         <v>23</v>
       </c>
@@ -2096,8 +2116,8 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="22"/>
-      <c r="B19" s="19"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="13" t="s">
         <v>43</v>
       </c>
@@ -2571,65 +2591,74 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{181693DF-27B0-4E27-A483-E7C504AA61A6}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="18" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="E1" s="18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="20" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="25"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="25"/>
+      <c r="D3" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="21"/>
+      <c r="D4" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>